<commit_message>
Agrego botón para simulación por forma reciente
</commit_message>
<xml_diff>
--- a/Ligas/Liga_ecuador_2025.xlsx
+++ b/Ligas/Liga_ecuador_2025.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raque\Desktop\ligas_datas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raque\Desktop\ligas_datas\rockongo_web\Ligas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4502E12D-92A0-45CC-9EEF-612C1AB9A172}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54FC91ED-3580-4EC4-B7C8-79CB96D08B27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="883" uniqueCount="142">
   <si>
     <t>Fecha</t>
   </si>
@@ -440,6 +440,12 @@
   </si>
   <si>
     <t>2025-07-05</t>
+  </si>
+  <si>
+    <t>Empate</t>
+  </si>
+  <si>
+    <t>Resultado</t>
   </si>
 </sst>
 </file>
@@ -812,10 +818,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R147"/>
+  <dimension ref="A1:S147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B118" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="R133" sqref="R133"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="V11" sqref="V11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -839,7 +845,7 @@
     <col min="18" max="18" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -894,8 +900,11 @@
       <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S1" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>18</v>
       </c>
@@ -950,8 +959,11 @@
       <c r="R2" s="2">
         <v>57</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>18</v>
       </c>
@@ -1006,8 +1018,11 @@
       <c r="R3" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
@@ -1062,8 +1077,11 @@
       <c r="R4" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>28</v>
       </c>
@@ -1118,8 +1136,11 @@
       <c r="R5" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>28</v>
       </c>
@@ -1174,8 +1195,11 @@
       <c r="R6" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S6" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>28</v>
       </c>
@@ -1230,8 +1254,11 @@
       <c r="R7" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>28</v>
       </c>
@@ -1286,8 +1313,11 @@
       <c r="R8" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>45</v>
       </c>
@@ -1342,8 +1372,11 @@
       <c r="R9" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>48</v>
       </c>
@@ -1398,8 +1431,11 @@
       <c r="R10" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>48</v>
       </c>
@@ -1454,8 +1490,11 @@
       <c r="R11" s="2" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>48</v>
       </c>
@@ -1510,8 +1549,11 @@
       <c r="R12" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>55</v>
       </c>
@@ -1566,8 +1608,11 @@
       <c r="R13" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S13" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>55</v>
       </c>
@@ -1622,8 +1667,11 @@
       <c r="R14" s="2" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S14" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>55</v>
       </c>
@@ -1678,8 +1726,11 @@
       <c r="R15" s="2" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S15" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>55</v>
       </c>
@@ -1734,8 +1785,11 @@
       <c r="R16" s="2" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S16" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>64</v>
       </c>
@@ -1790,8 +1844,11 @@
       <c r="R17" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S17" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>65</v>
       </c>
@@ -1846,8 +1903,11 @@
       <c r="R18" s="2" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S18" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>65</v>
       </c>
@@ -1902,8 +1962,11 @@
       <c r="R19" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S19" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>65</v>
       </c>
@@ -1958,8 +2021,11 @@
       <c r="R20" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S20" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>68</v>
       </c>
@@ -2014,8 +2080,11 @@
       <c r="R21" s="2" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S21" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>68</v>
       </c>
@@ -2070,8 +2139,11 @@
       <c r="R22" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S22" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>68</v>
       </c>
@@ -2126,8 +2198,11 @@
       <c r="R23" s="2" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S23" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>68</v>
       </c>
@@ -2182,8 +2257,11 @@
       <c r="R24" s="2" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S24" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>71</v>
       </c>
@@ -2238,8 +2316,11 @@
       <c r="R25" s="2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S25" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>74</v>
       </c>
@@ -2294,8 +2375,11 @@
       <c r="R26" s="2" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S26" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>74</v>
       </c>
@@ -2350,8 +2434,11 @@
       <c r="R27" s="2" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S27" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>74</v>
       </c>
@@ -2406,8 +2493,11 @@
       <c r="R28" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S28" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>77</v>
       </c>
@@ -2462,8 +2552,11 @@
       <c r="R29" s="2" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S29" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>77</v>
       </c>
@@ -2518,8 +2611,11 @@
       <c r="R30" s="2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S30" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>77</v>
       </c>
@@ -2574,8 +2670,11 @@
       <c r="R31" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S31" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>77</v>
       </c>
@@ -2630,8 +2729,11 @@
       <c r="R32" s="2" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S32" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>82</v>
       </c>
@@ -2686,8 +2788,11 @@
       <c r="R33" s="2" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S33" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>85</v>
       </c>
@@ -2742,8 +2847,11 @@
       <c r="R34" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S34" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>85</v>
       </c>
@@ -2798,8 +2906,11 @@
       <c r="R35" s="2" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S35" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>85</v>
       </c>
@@ -2854,8 +2965,11 @@
       <c r="R36" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S36" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>88</v>
       </c>
@@ -2910,8 +3024,11 @@
       <c r="R37" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S37" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>88</v>
       </c>
@@ -2966,8 +3083,11 @@
       <c r="R38" s="2" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S38" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>88</v>
       </c>
@@ -3022,8 +3142,11 @@
       <c r="R39" s="2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S39" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>88</v>
       </c>
@@ -3078,8 +3201,11 @@
       <c r="R40" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S40" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>91</v>
       </c>
@@ -3134,8 +3260,11 @@
       <c r="R41" s="2" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S41" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>92</v>
       </c>
@@ -3190,8 +3319,11 @@
       <c r="R42" s="2">
         <v>48</v>
       </c>
-    </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S42" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>93</v>
       </c>
@@ -3246,8 +3378,11 @@
       <c r="R43" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S43" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>93</v>
       </c>
@@ -3302,8 +3437,11 @@
       <c r="R44" s="2" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S44" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>93</v>
       </c>
@@ -3358,8 +3496,11 @@
       <c r="R45" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S45" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>94</v>
       </c>
@@ -3414,8 +3555,11 @@
       <c r="R46" s="2" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S46" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>94</v>
       </c>
@@ -3470,8 +3614,11 @@
       <c r="R47" s="2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S47" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>94</v>
       </c>
@@ -3526,8 +3673,11 @@
       <c r="R48" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S48" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>94</v>
       </c>
@@ -3582,8 +3732,11 @@
       <c r="R49" s="2" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S49" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>95</v>
       </c>
@@ -3638,8 +3791,11 @@
       <c r="R50" s="2" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S50" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>95</v>
       </c>
@@ -3694,8 +3850,11 @@
       <c r="R51" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S51" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>95</v>
       </c>
@@ -3750,8 +3909,11 @@
       <c r="R52" s="2" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S52" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>96</v>
       </c>
@@ -3806,8 +3968,11 @@
       <c r="R53" s="2" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S53" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>96</v>
       </c>
@@ -3862,8 +4027,11 @@
       <c r="R54" s="2" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S54" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="55" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>96</v>
       </c>
@@ -3918,8 +4086,11 @@
       <c r="R55" s="2" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S55" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>96</v>
       </c>
@@ -3974,8 +4145,11 @@
       <c r="R56" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S56" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="57" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>97</v>
       </c>
@@ -4030,8 +4204,11 @@
       <c r="R57" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S57" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>97</v>
       </c>
@@ -4086,8 +4263,11 @@
       <c r="R58" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S58" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>98</v>
       </c>
@@ -4142,8 +4322,11 @@
       <c r="R59" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S59" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>99</v>
       </c>
@@ -4198,8 +4381,11 @@
       <c r="R60" s="2" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S60" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="61" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>100</v>
       </c>
@@ -4254,8 +4440,11 @@
       <c r="R61" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S61" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>100</v>
       </c>
@@ -4310,8 +4499,11 @@
       <c r="R62" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S62" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>101</v>
       </c>
@@ -4366,8 +4558,11 @@
       <c r="R63" s="2" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S63" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>102</v>
       </c>
@@ -4422,8 +4617,11 @@
       <c r="R64" s="2" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S64" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>103</v>
       </c>
@@ -4478,8 +4676,11 @@
       <c r="R65" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S65" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>104</v>
       </c>
@@ -4534,8 +4735,11 @@
       <c r="R66" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S66" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>104</v>
       </c>
@@ -4590,8 +4794,11 @@
       <c r="R67" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S67" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>104</v>
       </c>
@@ -4646,8 +4853,11 @@
       <c r="R68" s="2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S68" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>105</v>
       </c>
@@ -4702,8 +4912,11 @@
       <c r="R69" s="2" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S69" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>105</v>
       </c>
@@ -4758,8 +4971,11 @@
       <c r="R70" s="2" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S70" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>105</v>
       </c>
@@ -4814,8 +5030,11 @@
       <c r="R71" s="2" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S71" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>105</v>
       </c>
@@ -4870,8 +5089,11 @@
       <c r="R72" s="2" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S72" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="73" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>106</v>
       </c>
@@ -4926,8 +5148,11 @@
       <c r="R73" s="2" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S73" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>106</v>
       </c>
@@ -4982,8 +5207,11 @@
       <c r="R74" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S74" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>106</v>
       </c>
@@ -5038,8 +5266,11 @@
       <c r="R75" s="2" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S75" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="76" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>107</v>
       </c>
@@ -5094,8 +5325,11 @@
       <c r="R76" s="2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S76" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>107</v>
       </c>
@@ -5150,8 +5384,11 @@
       <c r="R77" s="2" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S77" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>107</v>
       </c>
@@ -5206,8 +5443,11 @@
       <c r="R78" s="2" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S78" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>107</v>
       </c>
@@ -5262,8 +5502,11 @@
       <c r="R79" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S79" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>108</v>
       </c>
@@ -5318,8 +5561,11 @@
       <c r="R80" s="2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S80" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>109</v>
       </c>
@@ -5374,8 +5620,11 @@
       <c r="R81" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S81" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>109</v>
       </c>
@@ -5430,8 +5679,11 @@
       <c r="R82" s="2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="83" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S82" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="83" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>109</v>
       </c>
@@ -5486,8 +5738,11 @@
       <c r="R83" s="2" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="84" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S83" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="84" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
         <v>110</v>
       </c>
@@ -5542,8 +5797,11 @@
       <c r="R84" s="2" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="85" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S84" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
         <v>110</v>
       </c>
@@ -5598,8 +5856,11 @@
       <c r="R85" s="2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="86" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S85" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="86" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
         <v>110</v>
       </c>
@@ -5654,8 +5915,11 @@
       <c r="R86" s="2" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="87" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S86" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>110</v>
       </c>
@@ -5710,8 +5974,11 @@
       <c r="R87" s="2">
         <v>33</v>
       </c>
-    </row>
-    <row r="88" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S87" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
         <v>111</v>
       </c>
@@ -5766,8 +6033,11 @@
       <c r="R88" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="89" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S88" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
         <v>112</v>
       </c>
@@ -5822,8 +6092,11 @@
       <c r="R89" s="2" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="90" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S89" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
         <v>112</v>
       </c>
@@ -5878,8 +6151,11 @@
       <c r="R90" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="91" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S90" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
         <v>112</v>
       </c>
@@ -5934,8 +6210,11 @@
       <c r="R91" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="92" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S91" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
         <v>113</v>
       </c>
@@ -5990,8 +6269,11 @@
       <c r="R92" s="2" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="93" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S92" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
         <v>113</v>
       </c>
@@ -6046,8 +6328,11 @@
       <c r="R93" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="94" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S93" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
         <v>113</v>
       </c>
@@ -6102,8 +6387,11 @@
       <c r="R94" s="2" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="95" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S94" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="95" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
         <v>113</v>
       </c>
@@ -6158,8 +6446,11 @@
       <c r="R95" s="2" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="96" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S95" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
         <v>114</v>
       </c>
@@ -6214,8 +6505,11 @@
       <c r="R96" s="2" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="97" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S96" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
         <v>115</v>
       </c>
@@ -6270,8 +6564,11 @@
       <c r="R97" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="98" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S97" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
         <v>115</v>
       </c>
@@ -6326,8 +6623,11 @@
       <c r="R98" s="2" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="99" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S98" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="99" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
         <v>115</v>
       </c>
@@ -6382,8 +6682,11 @@
       <c r="R99" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="100" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S99" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
         <v>116</v>
       </c>
@@ -6438,8 +6741,11 @@
       <c r="R100" s="2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="101" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S100" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="101" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
         <v>116</v>
       </c>
@@ -6494,8 +6800,11 @@
       <c r="R101" s="2" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="102" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S101" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
         <v>116</v>
       </c>
@@ -6550,8 +6859,11 @@
       <c r="R102" s="2" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="103" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S102" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
         <v>116</v>
       </c>
@@ -6606,8 +6918,11 @@
       <c r="R103" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="104" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S103" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A104" s="2" t="s">
         <v>117</v>
       </c>
@@ -6662,8 +6977,11 @@
       <c r="R104" s="2" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="105" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S104" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="105" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
         <v>118</v>
       </c>
@@ -6718,8 +7036,11 @@
       <c r="R105" s="2" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="106" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S105" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
         <v>121</v>
       </c>
@@ -6774,8 +7095,11 @@
       <c r="R106" s="2" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="107" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S106" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="107" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A107" s="2" t="s">
         <v>121</v>
       </c>
@@ -6830,8 +7154,11 @@
       <c r="R107" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="108" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S107" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="108" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A108" s="2" t="s">
         <v>121</v>
       </c>
@@ -6886,8 +7213,11 @@
       <c r="R108" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="109" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S108" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
         <v>122</v>
       </c>
@@ -6942,8 +7272,11 @@
       <c r="R109" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="110" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S109" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A110" s="2" t="s">
         <v>122</v>
       </c>
@@ -6998,8 +7331,11 @@
       <c r="R110" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="111" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S110" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="111" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A111" s="2" t="s">
         <v>122</v>
       </c>
@@ -7054,8 +7390,11 @@
       <c r="R111" s="2" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="112" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S111" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="112" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A112" s="2" t="s">
         <v>122</v>
       </c>
@@ -7110,8 +7449,11 @@
       <c r="R112" s="2" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="113" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S112" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
         <v>123</v>
       </c>
@@ -7166,8 +7508,11 @@
       <c r="R113" s="2" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="114" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S113" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="114" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A114" s="2" t="s">
         <v>123</v>
       </c>
@@ -7222,8 +7567,11 @@
       <c r="R114" s="2" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="115" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S114" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
         <v>123</v>
       </c>
@@ -7278,8 +7626,11 @@
       <c r="R115" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="116" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S115" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="116" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
         <v>126</v>
       </c>
@@ -7334,8 +7685,11 @@
       <c r="R116" s="2" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="117" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S116" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A117" s="2" t="s">
         <v>126</v>
       </c>
@@ -7390,8 +7744,11 @@
       <c r="R117" s="2" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="118" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S117" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="118" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A118" s="2" t="s">
         <v>126</v>
       </c>
@@ -7446,8 +7803,11 @@
       <c r="R118" s="2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="119" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S118" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A119" s="2" t="s">
         <v>126</v>
       </c>
@@ -7502,8 +7862,11 @@
       <c r="R119" s="2" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="120" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S119" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A120" s="2" t="s">
         <v>127</v>
       </c>
@@ -7558,8 +7921,11 @@
       <c r="R120" s="2" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="121" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S120" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A121" s="2" t="s">
         <v>128</v>
       </c>
@@ -7614,8 +7980,11 @@
       <c r="R121" s="2" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="122" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S121" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="122" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A122" s="2" t="s">
         <v>128</v>
       </c>
@@ -7670,8 +8039,11 @@
       <c r="R122" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="123" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S122" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="123" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A123" s="2" t="s">
         <v>129</v>
       </c>
@@ -7726,8 +8098,11 @@
       <c r="R123" s="2">
         <v>72</v>
       </c>
-    </row>
-    <row r="124" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S123" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="124" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A124" s="2" t="s">
         <v>129</v>
       </c>
@@ -7782,8 +8157,11 @@
       <c r="R124" s="2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="125" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S124" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="125" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A125" s="2" t="s">
         <v>129</v>
       </c>
@@ -7838,8 +8216,11 @@
       <c r="R125" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="126" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S125" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A126" s="2" t="s">
         <v>129</v>
       </c>
@@ -7894,8 +8275,11 @@
       <c r="R126" s="2" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="127" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S126" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A127" s="2" t="s">
         <v>130</v>
       </c>
@@ -7950,8 +8334,11 @@
       <c r="R127" s="2" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="128" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S127" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A128" s="2" t="s">
         <v>131</v>
       </c>
@@ -8006,8 +8393,11 @@
       <c r="R128" s="2">
         <v>36</v>
       </c>
-    </row>
-    <row r="129" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S128" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A129" s="2" t="s">
         <v>132</v>
       </c>
@@ -8062,8 +8452,11 @@
       <c r="R129" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="130" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S129" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A130" s="2" t="s">
         <v>132</v>
       </c>
@@ -8118,8 +8511,11 @@
       <c r="R130" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="131" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S130" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="131" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A131" s="2" t="s">
         <v>132</v>
       </c>
@@ -8174,8 +8570,11 @@
       <c r="R131" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="132" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S131" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="132" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A132" s="2" t="s">
         <v>133</v>
       </c>
@@ -8230,8 +8629,11 @@
       <c r="R132" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="133" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S132" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A133" s="2" t="s">
         <v>133</v>
       </c>
@@ -8286,8 +8688,11 @@
       <c r="R133" s="2">
         <v>42</v>
       </c>
-    </row>
-    <row r="134" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S133" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="134" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A134" s="2" t="s">
         <v>133</v>
       </c>
@@ -8342,8 +8747,11 @@
       <c r="R134" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="135" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S134" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="135" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A135" s="2" t="s">
         <v>133</v>
       </c>
@@ -8398,8 +8806,11 @@
       <c r="R135" s="2" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="136" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S135" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="136" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A136" s="2" t="s">
         <v>134</v>
       </c>
@@ -8454,8 +8865,11 @@
       <c r="R136" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="137" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S136" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="137" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A137" s="2" t="s">
         <v>135</v>
       </c>
@@ -8510,8 +8924,11 @@
       <c r="R137" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="138" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S137" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="138" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A138" s="2" t="s">
         <v>136</v>
       </c>
@@ -8566,8 +8983,11 @@
       <c r="R138" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="139" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S138" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A139" s="2" t="s">
         <v>136</v>
       </c>
@@ -8622,8 +9042,11 @@
       <c r="R139" s="2" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="140" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S139" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A140" s="2" t="s">
         <v>136</v>
       </c>
@@ -8678,8 +9101,11 @@
       <c r="R140" s="2" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="141" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S140" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="141" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A141" s="2" t="s">
         <v>137</v>
       </c>
@@ -8734,8 +9160,11 @@
       <c r="R141" s="2" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="142" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S141" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A142" s="2" t="s">
         <v>137</v>
       </c>
@@ -8790,8 +9219,11 @@
       <c r="R142" s="2" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="143" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S142" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="143" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A143" s="2" t="s">
         <v>137</v>
       </c>
@@ -8846,8 +9278,11 @@
       <c r="R143" s="2" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="144" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S143" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="144" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A144" s="2" t="s">
         <v>137</v>
       </c>
@@ -8902,8 +9337,11 @@
       <c r="R144" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="145" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S144" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="145" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A145" s="2" t="s">
         <v>138</v>
       </c>
@@ -8958,8 +9396,11 @@
       <c r="R145" s="2" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="146" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S145" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="146" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A146" s="2" t="s">
         <v>139</v>
       </c>
@@ -9014,8 +9455,11 @@
       <c r="R146" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="147" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S146" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A147" s="2" t="s">
         <v>139</v>
       </c>
@@ -9069,6 +9513,9 @@
       </c>
       <c r="R147" s="2" t="s">
         <v>124</v>
+      </c>
+      <c r="S147" t="s">
+        <v>140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Agregado orden alfabético a diccionario de ligas en app.py
</commit_message>
<xml_diff>
--- a/Ligas/Liga_ecuador_2025.xlsx
+++ b/Ligas/Liga_ecuador_2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raque\Desktop\ligas_datas\rockongo_web\Ligas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1A25B12-8ED1-4408-8806-E923F69E97EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06504EBB-157A-4D31-9A82-DA38F6033A06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -681,13 +681,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A137" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="Q153" sqref="Q153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">

</xml_diff>